<commit_message>
plantilla análisis de información
</commit_message>
<xml_diff>
--- a/plantilla-para-analisis-comprension-de-textos-4-dimensiones-3-indicadores-24-preguntas.xlsx
+++ b/plantilla-para-analisis-comprension-de-textos-4-dimensiones-3-indicadores-24-preguntas.xlsx
@@ -707,119 +707,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -828,24 +723,6 @@
     <xf numFmtId="9" fontId="7" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="7" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="7" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -889,6 +766,129 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="5" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1286,12 +1286,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-1981547536"/>
-        <c:axId val="-2044323520"/>
+        <c:axId val="-2071436880"/>
+        <c:axId val="-2090855136"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-1981547536"/>
+        <c:axId val="-2071436880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1328,7 +1328,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2044323520"/>
+        <c:crossAx val="-2090855136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1336,7 +1336,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2044323520"/>
+        <c:axId val="-2090855136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1443,7 +1443,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1981547536"/>
+        <c:crossAx val="-2071436880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1782,12 +1782,12 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:shape val="box"/>
-        <c:axId val="-2053301184"/>
-        <c:axId val="-2053732096"/>
+        <c:axId val="-2066474976"/>
+        <c:axId val="-2066471744"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-2053301184"/>
+        <c:axId val="-2066474976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1830,7 +1830,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2053732096"/>
+        <c:crossAx val="-2066471744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1838,7 +1838,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2053732096"/>
+        <c:axId val="-2066471744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1889,7 +1889,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2053301184"/>
+        <c:crossAx val="-2066474976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2181,12 +2181,12 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:shape val="box"/>
-        <c:axId val="-2053851472"/>
-        <c:axId val="-2054043552"/>
+        <c:axId val="-2066734912"/>
+        <c:axId val="-2066731680"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-2053851472"/>
+        <c:axId val="-2066734912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2229,7 +2229,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2054043552"/>
+        <c:crossAx val="-2066731680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2237,7 +2237,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2054043552"/>
+        <c:axId val="-2066731680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2288,7 +2288,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2053851472"/>
+        <c:crossAx val="-2066734912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2575,12 +2575,12 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:shape val="box"/>
-        <c:axId val="-2053792816"/>
-        <c:axId val="-2053854656"/>
+        <c:axId val="-2066706032"/>
+        <c:axId val="-2066702800"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-2053792816"/>
+        <c:axId val="-2066706032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2623,7 +2623,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2053854656"/>
+        <c:crossAx val="-2066702800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2631,7 +2631,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2053854656"/>
+        <c:axId val="-2066702800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2682,7 +2682,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2053792816"/>
+        <c:crossAx val="-2066706032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2986,12 +2986,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-2028297008"/>
-        <c:axId val="-2053870240"/>
+        <c:axId val="-2046445104"/>
+        <c:axId val="-2046441744"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-2028297008"/>
+        <c:axId val="-2046445104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3028,7 +3028,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2053870240"/>
+        <c:crossAx val="-2046441744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3036,7 +3036,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2053870240"/>
+        <c:axId val="-2046441744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3087,7 +3087,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2028297008"/>
+        <c:crossAx val="-2046445104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3386,12 +3386,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-2082206640"/>
-        <c:axId val="-2080408624"/>
+        <c:axId val="-2071834256"/>
+        <c:axId val="-2094059040"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-2082206640"/>
+        <c:axId val="-2071834256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3428,7 +3428,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2080408624"/>
+        <c:crossAx val="-2094059040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3436,7 +3436,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2080408624"/>
+        <c:axId val="-2094059040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3487,7 +3487,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082206640"/>
+        <c:crossAx val="-2071834256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3905,12 +3905,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-1985209504"/>
-        <c:axId val="-1985829264"/>
+        <c:axId val="-2069517056"/>
+        <c:axId val="-2069517600"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-1985209504"/>
+        <c:axId val="-2069517056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3947,7 +3947,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1985829264"/>
+        <c:crossAx val="-2069517600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3955,7 +3955,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1985829264"/>
+        <c:axId val="-2069517600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4062,7 +4062,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1985209504"/>
+        <c:crossAx val="-2069517056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4516,12 +4516,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-2005111984"/>
-        <c:axId val="-1988274752"/>
+        <c:axId val="-2069859984"/>
+        <c:axId val="-2069856560"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-2005111984"/>
+        <c:axId val="-2069859984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4558,7 +4558,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1988274752"/>
+        <c:crossAx val="-2069856560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4566,7 +4566,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1988274752"/>
+        <c:axId val="-2069856560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4673,7 +4673,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2005111984"/>
+        <c:crossAx val="-2069859984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5130,12 +5130,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-1994285152"/>
-        <c:axId val="-1995947952"/>
+        <c:axId val="-2069804960"/>
+        <c:axId val="-2069801536"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-1994285152"/>
+        <c:axId val="-2069804960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5172,7 +5172,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1995947952"/>
+        <c:crossAx val="-2069801536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5180,7 +5180,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1995947952"/>
+        <c:axId val="-2069801536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5287,7 +5287,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1994285152"/>
+        <c:crossAx val="-2069804960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5744,12 +5744,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-1962452288"/>
-        <c:axId val="-2039792016"/>
+        <c:axId val="-2069755232"/>
+        <c:axId val="-2069751808"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-1962452288"/>
+        <c:axId val="-2069755232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5786,7 +5786,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2039792016"/>
+        <c:crossAx val="-2069751808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5794,7 +5794,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2039792016"/>
+        <c:axId val="-2069751808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5901,7 +5901,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1962452288"/>
+        <c:crossAx val="-2069755232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6358,12 +6358,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-1984296912"/>
-        <c:axId val="-1983860960"/>
+        <c:axId val="-2069701904"/>
+        <c:axId val="-2069698480"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-1984296912"/>
+        <c:axId val="-2069701904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6400,7 +6400,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1983860960"/>
+        <c:crossAx val="-2069698480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6408,7 +6408,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1983860960"/>
+        <c:axId val="-2069698480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6515,7 +6515,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1984296912"/>
+        <c:crossAx val="-2069701904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6976,12 +6976,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-1993041584"/>
-        <c:axId val="-1994320560"/>
+        <c:axId val="-2071805872"/>
+        <c:axId val="-2071799344"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-1993041584"/>
+        <c:axId val="-2071805872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7018,7 +7018,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1994320560"/>
+        <c:crossAx val="-2071799344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7026,7 +7026,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1994320560"/>
+        <c:axId val="-2071799344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7133,7 +7133,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1993041584"/>
+        <c:crossAx val="-2071805872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7820,11 +7820,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2053212544"/>
-        <c:axId val="-2053218416"/>
+        <c:axId val="-2069723056"/>
+        <c:axId val="-2069680192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2053212544"/>
+        <c:axId val="-2069723056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7881,12 +7881,12 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2053218416"/>
+        <c:crossAx val="-2069680192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2053218416"/>
+        <c:axId val="-2069680192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7943,7 +7943,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2053212544"/>
+        <c:crossAx val="-2069723056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8623,11 +8623,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2028607312"/>
-        <c:axId val="-2028603904"/>
+        <c:axId val="-2046410704"/>
+        <c:axId val="-2046408256"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2028607312"/>
+        <c:axId val="-2046410704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8684,12 +8684,12 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2028603904"/>
+        <c:crossAx val="-2046408256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2028603904"/>
+        <c:axId val="-2046408256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8746,7 +8746,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2028607312"/>
+        <c:crossAx val="-2046410704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9196,12 +9196,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="1829282688"/>
-        <c:axId val="1829035200"/>
+        <c:axId val="-2071657888"/>
+        <c:axId val="-2071654464"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1829282688"/>
+        <c:axId val="-2071657888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9238,7 +9238,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1829035200"/>
+        <c:crossAx val="-2071654464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9246,7 +9246,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1829035200"/>
+        <c:axId val="-2071654464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9353,7 +9353,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1829282688"/>
+        <c:crossAx val="-2071657888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9810,12 +9810,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="1835862272"/>
-        <c:axId val="1835494800"/>
+        <c:axId val="-2071604912"/>
+        <c:axId val="-2071601488"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1835862272"/>
+        <c:axId val="-2071604912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9852,7 +9852,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1835494800"/>
+        <c:crossAx val="-2071601488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9860,7 +9860,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1835494800"/>
+        <c:axId val="-2071601488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9967,7 +9967,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1835862272"/>
+        <c:crossAx val="-2071604912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10358,12 +10358,12 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:shape val="box"/>
-        <c:axId val="-2005826576"/>
-        <c:axId val="-2005823312"/>
+        <c:axId val="-2070907088"/>
+        <c:axId val="-2070903808"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-2005826576"/>
+        <c:axId val="-2070907088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10406,7 +10406,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2005823312"/>
+        <c:crossAx val="-2070903808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10414,7 +10414,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2005823312"/>
+        <c:axId val="-2070903808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10465,7 +10465,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2005826576"/>
+        <c:crossAx val="-2070907088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10757,12 +10757,12 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:shape val="box"/>
-        <c:axId val="-2088633360"/>
-        <c:axId val="-2088639152"/>
+        <c:axId val="-2070885920"/>
+        <c:axId val="-2070882688"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-2088633360"/>
+        <c:axId val="-2070885920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10805,7 +10805,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2088639152"/>
+        <c:crossAx val="-2070882688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10813,7 +10813,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2088639152"/>
+        <c:axId val="-2070882688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10864,7 +10864,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2088633360"/>
+        <c:crossAx val="-2070885920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11160,12 +11160,12 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:shape val="box"/>
-        <c:axId val="-2005557648"/>
-        <c:axId val="-2005559952"/>
+        <c:axId val="-2066556912"/>
+        <c:axId val="-2066553680"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-2005557648"/>
+        <c:axId val="-2066556912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11208,7 +11208,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2005559952"/>
+        <c:crossAx val="-2066553680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11216,7 +11216,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2005559952"/>
+        <c:axId val="-2066553680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11267,7 +11267,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2005557648"/>
+        <c:crossAx val="-2066556912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11567,12 +11567,12 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:shape val="box"/>
-        <c:axId val="-2088570800"/>
-        <c:axId val="-2088494928"/>
+        <c:axId val="-2066575952"/>
+        <c:axId val="-2066572720"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-2088570800"/>
+        <c:axId val="-2066575952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11615,7 +11615,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2088494928"/>
+        <c:crossAx val="-2066572720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11623,7 +11623,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2088494928"/>
+        <c:axId val="-2066572720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11674,7 +11674,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2088570800"/>
+        <c:crossAx val="-2066575952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11966,12 +11966,12 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:shape val="box"/>
-        <c:axId val="-2053975648"/>
-        <c:axId val="-2053136432"/>
+        <c:axId val="-2089685104"/>
+        <c:axId val="-2089681872"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-2053975648"/>
+        <c:axId val="-2089685104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12014,7 +12014,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2053136432"/>
+        <c:crossAx val="-2089681872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12022,7 +12022,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2053136432"/>
+        <c:axId val="-2089681872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12073,7 +12073,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2053975648"/>
+        <c:crossAx val="-2089685104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -23597,7 +23597,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23633,7 +23633,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23669,7 +23669,7 @@
         <xdr:cNvPr id="4" name="Gráfico 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23705,7 +23705,7 @@
         <xdr:cNvPr id="5" name="Gráfico 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23741,7 +23741,7 @@
         <xdr:cNvPr id="6" name="Gráfico 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23777,7 +23777,7 @@
         <xdr:cNvPr id="7" name="Gráfico 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23813,7 +23813,7 @@
         <xdr:cNvPr id="8" name="Gráfico 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23849,7 +23849,7 @@
         <xdr:cNvPr id="9" name="Gráfico 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000009000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000009000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23885,7 +23885,7 @@
         <xdr:cNvPr id="10" name="Gráfico 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C60FEBB-1128-40F0-80C3-0A870DCF4D6E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9C60FEBB-1128-40F0-80C3-0A870DCF4D6E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -23921,7 +23921,7 @@
         <xdr:cNvPr id="11" name="Gráfico 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{811EC65F-EA02-4407-B17A-A26F938CD13D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{811EC65F-EA02-4407-B17A-A26F938CD13D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24112,7 +24112,7 @@
         <xdr:cNvPr id="4" name="Gráfico 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24153,7 +24153,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -24486,113 +24486,113 @@
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A1" s="33"/>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="49" t="s">
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="50" t="s">
+      <c r="K1" s="83"/>
+      <c r="L1" s="83"/>
+      <c r="M1" s="83"/>
+      <c r="N1" s="83"/>
+      <c r="O1" s="83"/>
+      <c r="P1" s="83"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="50"/>
-      <c r="T1" s="50"/>
-      <c r="U1" s="50"/>
-      <c r="V1" s="50"/>
-      <c r="W1" s="50"/>
-      <c r="X1" s="50"/>
-      <c r="Y1" s="50"/>
-      <c r="Z1" s="58" t="s">
+      <c r="S1" s="84"/>
+      <c r="T1" s="84"/>
+      <c r="U1" s="84"/>
+      <c r="V1" s="84"/>
+      <c r="W1" s="84"/>
+      <c r="X1" s="84"/>
+      <c r="Y1" s="84"/>
+      <c r="Z1" s="76" t="s">
         <v>75</v>
       </c>
-      <c r="AA1" s="58"/>
-      <c r="AB1" s="58"/>
-      <c r="AC1" s="58"/>
-      <c r="AD1" s="58"/>
-      <c r="AE1" s="58"/>
-      <c r="AF1" s="58"/>
-      <c r="AG1" s="58"/>
-      <c r="AH1" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI1" s="51" t="s">
+      <c r="AA1" s="76"/>
+      <c r="AB1" s="76"/>
+      <c r="AC1" s="76"/>
+      <c r="AD1" s="76"/>
+      <c r="AE1" s="76"/>
+      <c r="AF1" s="76"/>
+      <c r="AG1" s="76"/>
+      <c r="AH1" s="85" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI1" s="85" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2" s="33"/>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="53"/>
-      <c r="D2" s="52" t="s">
+      <c r="C2" s="75"/>
+      <c r="D2" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="53"/>
-      <c r="F2" s="52" t="s">
+      <c r="E2" s="75"/>
+      <c r="F2" s="74" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="53"/>
+      <c r="G2" s="75"/>
       <c r="H2" s="35"/>
       <c r="I2" s="35"/>
-      <c r="J2" s="54" t="s">
+      <c r="J2" s="86" t="s">
         <v>50</v>
       </c>
-      <c r="K2" s="55"/>
-      <c r="L2" s="54" t="s">
+      <c r="K2" s="87"/>
+      <c r="L2" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="M2" s="55"/>
-      <c r="N2" s="54" t="s">
+      <c r="M2" s="87"/>
+      <c r="N2" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="O2" s="55"/>
+      <c r="O2" s="87"/>
       <c r="P2" s="36"/>
       <c r="Q2" s="36"/>
-      <c r="R2" s="56" t="s">
+      <c r="R2" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="S2" s="57"/>
-      <c r="T2" s="56" t="s">
+      <c r="S2" s="89"/>
+      <c r="T2" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="U2" s="57"/>
-      <c r="V2" s="56" t="s">
+      <c r="U2" s="89"/>
+      <c r="V2" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="W2" s="57"/>
+      <c r="W2" s="89"/>
       <c r="X2" s="37"/>
       <c r="Y2" s="37"/>
-      <c r="Z2" s="52" t="s">
+      <c r="Z2" s="74" t="s">
         <v>47</v>
       </c>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="52" t="s">
+      <c r="AA2" s="75"/>
+      <c r="AB2" s="74" t="s">
         <v>48</v>
       </c>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="52" t="s">
+      <c r="AC2" s="75"/>
+      <c r="AD2" s="74" t="s">
         <v>49</v>
       </c>
-      <c r="AE2" s="53"/>
+      <c r="AE2" s="75"/>
       <c r="AF2" s="35"/>
       <c r="AG2" s="35"/>
-      <c r="AH2" s="51"/>
-      <c r="AI2" s="51"/>
+      <c r="AH2" s="85"/>
+      <c r="AI2" s="85"/>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3" s="33" t="s">
@@ -24694,8 +24694,8 @@
       <c r="AG3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="AH3" s="51"/>
-      <c r="AI3" s="51"/>
+      <c r="AH3" s="85"/>
+      <c r="AI3" s="85"/>
       <c r="AK3" s="33" t="s">
         <v>11</v>
       </c>
@@ -28345,8 +28345,8 @@
         <f>SUM(G4:G33)</f>
         <v>18</v>
       </c>
-      <c r="H34" s="100"/>
-      <c r="I34" s="101"/>
+      <c r="H34" s="59"/>
+      <c r="I34" s="60"/>
       <c r="J34" s="46">
         <f t="shared" ref="J34:O34" si="11">SUM(J4:J33)</f>
         <v>16</v>
@@ -28371,8 +28371,8 @@
         <f t="shared" si="11"/>
         <v>18</v>
       </c>
-      <c r="P34" s="106"/>
-      <c r="Q34" s="107"/>
+      <c r="P34" s="65"/>
+      <c r="Q34" s="66"/>
       <c r="R34" s="47">
         <f>SUM(R4:R33)</f>
         <v>10</v>
@@ -28397,8 +28397,8 @@
         <f>SUM(W4:W33)</f>
         <v>12</v>
       </c>
-      <c r="X34" s="106"/>
-      <c r="Y34" s="107"/>
+      <c r="X34" s="65"/>
+      <c r="Y34" s="66"/>
       <c r="Z34" s="45">
         <f>SUM(Z4:Z33)</f>
         <v>14</v>
@@ -28423,218 +28423,199 @@
         <f>SUM(AE4:AE33)</f>
         <v>12</v>
       </c>
-      <c r="AF34" s="100"/>
-      <c r="AG34" s="112"/>
-      <c r="AH34" s="112"/>
-      <c r="AI34" s="101"/>
+      <c r="AF34" s="59"/>
+      <c r="AG34" s="71"/>
+      <c r="AH34" s="71"/>
+      <c r="AI34" s="60"/>
     </row>
-    <row r="35" spans="1:35" s="90" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="93" t="s">
+    <row r="35" spans="1:35" s="55" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="B35" s="89">
+      <c r="B35" s="54">
         <f>B34/$A$33</f>
         <v>0.6</v>
       </c>
-      <c r="C35" s="89">
+      <c r="C35" s="54">
         <f t="shared" ref="C35:G35" si="14">C34/$A$33</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D35" s="89">
+      <c r="D35" s="54">
         <f t="shared" si="14"/>
         <v>0.43333333333333335</v>
       </c>
-      <c r="E35" s="89">
+      <c r="E35" s="54">
         <f t="shared" si="14"/>
         <v>0.56666666666666665</v>
       </c>
-      <c r="F35" s="89">
+      <c r="F35" s="54">
         <f t="shared" si="14"/>
         <v>0.6333333333333333</v>
       </c>
-      <c r="G35" s="89">
+      <c r="G35" s="54">
         <f t="shared" si="14"/>
         <v>0.6</v>
       </c>
-      <c r="H35" s="102"/>
-      <c r="I35" s="103"/>
-      <c r="J35" s="91">
-        <f>J34/$A$33</f>
+      <c r="H35" s="61"/>
+      <c r="I35" s="62"/>
+      <c r="J35" s="56">
+        <f t="shared" ref="J35:O35" si="15">J34/$A$33</f>
         <v>0.53333333333333333</v>
       </c>
-      <c r="K35" s="91">
-        <f>K34/$A$33</f>
+      <c r="K35" s="56">
+        <f t="shared" si="15"/>
         <v>0.5</v>
       </c>
-      <c r="L35" s="91">
-        <f>L34/$A$33</f>
+      <c r="L35" s="56">
+        <f t="shared" si="15"/>
         <v>0.6</v>
       </c>
-      <c r="M35" s="91">
-        <f>M34/$A$33</f>
+      <c r="M35" s="56">
+        <f t="shared" si="15"/>
         <v>0.3</v>
       </c>
-      <c r="N35" s="91">
-        <f>N34/$A$33</f>
+      <c r="N35" s="56">
+        <f t="shared" si="15"/>
         <v>0.56666666666666665</v>
       </c>
-      <c r="O35" s="91">
-        <f>O34/$A$33</f>
+      <c r="O35" s="56">
+        <f t="shared" si="15"/>
         <v>0.6</v>
       </c>
-      <c r="P35" s="108"/>
-      <c r="Q35" s="109"/>
-      <c r="R35" s="92">
-        <f>R34/$A$33</f>
+      <c r="P35" s="67"/>
+      <c r="Q35" s="68"/>
+      <c r="R35" s="57">
+        <f t="shared" ref="R35:W35" si="16">R34/$A$33</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="S35" s="92">
-        <f>S34/$A$33</f>
+      <c r="S35" s="57">
+        <f t="shared" si="16"/>
         <v>0.36666666666666664</v>
       </c>
-      <c r="T35" s="92">
-        <f>T34/$A$33</f>
+      <c r="T35" s="57">
+        <f t="shared" si="16"/>
         <v>0.5</v>
       </c>
-      <c r="U35" s="92">
-        <f>U34/$A$33</f>
+      <c r="U35" s="57">
+        <f t="shared" si="16"/>
         <v>0.4</v>
       </c>
-      <c r="V35" s="92">
-        <f>V34/$A$33</f>
+      <c r="V35" s="57">
+        <f t="shared" si="16"/>
         <v>0.5</v>
       </c>
-      <c r="W35" s="92">
-        <f>W34/$A$33</f>
+      <c r="W35" s="57">
+        <f t="shared" si="16"/>
         <v>0.4</v>
       </c>
-      <c r="X35" s="108"/>
-      <c r="Y35" s="109"/>
-      <c r="Z35" s="89">
-        <f>Z34/$A$33</f>
+      <c r="X35" s="67"/>
+      <c r="Y35" s="68"/>
+      <c r="Z35" s="54">
+        <f t="shared" ref="Z35:AE35" si="17">Z34/$A$33</f>
         <v>0.46666666666666667</v>
       </c>
-      <c r="AA35" s="89">
-        <f>AA34/$A$33</f>
+      <c r="AA35" s="54">
+        <f t="shared" si="17"/>
         <v>0.43333333333333335</v>
       </c>
-      <c r="AB35" s="89">
-        <f>AB34/$A$33</f>
+      <c r="AB35" s="54">
+        <f t="shared" si="17"/>
         <v>0.36666666666666664</v>
       </c>
-      <c r="AC35" s="89">
-        <f>AC34/$A$33</f>
+      <c r="AC35" s="54">
+        <f t="shared" si="17"/>
         <v>0.4</v>
       </c>
-      <c r="AD35" s="89">
-        <f>AD34/$A$33</f>
+      <c r="AD35" s="54">
+        <f t="shared" si="17"/>
         <v>0.53333333333333333</v>
       </c>
-      <c r="AE35" s="89">
-        <f>AE34/$A$33</f>
+      <c r="AE35" s="54">
+        <f t="shared" si="17"/>
         <v>0.4</v>
       </c>
-      <c r="AF35" s="102"/>
-      <c r="AG35" s="113"/>
-      <c r="AH35" s="113"/>
-      <c r="AI35" s="103"/>
+      <c r="AF35" s="61"/>
+      <c r="AG35" s="72"/>
+      <c r="AH35" s="72"/>
+      <c r="AI35" s="62"/>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B36" s="94">
+      <c r="B36" s="77">
         <f>(B35+C35)/2</f>
         <v>0.46666666666666667</v>
       </c>
-      <c r="C36" s="95"/>
-      <c r="D36" s="94">
+      <c r="C36" s="78"/>
+      <c r="D36" s="77">
         <f>(D35+E35)/2</f>
         <v>0.5</v>
       </c>
-      <c r="E36" s="95"/>
-      <c r="F36" s="94">
+      <c r="E36" s="78"/>
+      <c r="F36" s="77">
         <f>(F35+G35)/2</f>
         <v>0.6166666666666667</v>
       </c>
-      <c r="G36" s="95"/>
-      <c r="H36" s="104"/>
-      <c r="I36" s="105"/>
-      <c r="J36" s="96">
+      <c r="G36" s="78"/>
+      <c r="H36" s="63"/>
+      <c r="I36" s="64"/>
+      <c r="J36" s="79">
         <f>(J35+K35)/2</f>
         <v>0.51666666666666661</v>
       </c>
-      <c r="K36" s="97"/>
-      <c r="L36" s="96">
+      <c r="K36" s="80"/>
+      <c r="L36" s="79">
         <f>(L35+M35)/2</f>
         <v>0.44999999999999996</v>
       </c>
-      <c r="M36" s="97"/>
-      <c r="N36" s="96">
+      <c r="M36" s="80"/>
+      <c r="N36" s="79">
         <f>(N35+O35)/2</f>
         <v>0.58333333333333326</v>
       </c>
-      <c r="O36" s="97"/>
-      <c r="P36" s="110"/>
-      <c r="Q36" s="111"/>
-      <c r="R36" s="98">
+      <c r="O36" s="80"/>
+      <c r="P36" s="69"/>
+      <c r="Q36" s="70"/>
+      <c r="R36" s="81">
         <f>(R35+S35)/2</f>
         <v>0.35</v>
       </c>
-      <c r="S36" s="99"/>
-      <c r="T36" s="98">
+      <c r="S36" s="82"/>
+      <c r="T36" s="81">
         <f>(T35+U35)/2</f>
         <v>0.45</v>
       </c>
-      <c r="U36" s="99"/>
-      <c r="V36" s="98">
+      <c r="U36" s="82"/>
+      <c r="V36" s="81">
         <f>(V35+W35)/2</f>
         <v>0.45</v>
       </c>
-      <c r="W36" s="99"/>
-      <c r="X36" s="110"/>
-      <c r="Y36" s="111"/>
-      <c r="Z36" s="94">
+      <c r="W36" s="82"/>
+      <c r="X36" s="69"/>
+      <c r="Y36" s="70"/>
+      <c r="Z36" s="77">
         <f>(Z35+AA35)/2</f>
         <v>0.45</v>
       </c>
-      <c r="AA36" s="95"/>
-      <c r="AB36" s="94">
+      <c r="AA36" s="78"/>
+      <c r="AB36" s="77">
         <f>(AB35+AC35)/2</f>
         <v>0.3833333333333333</v>
       </c>
-      <c r="AC36" s="95"/>
-      <c r="AD36" s="94">
+      <c r="AC36" s="78"/>
+      <c r="AD36" s="77">
         <f>(AD35+AE35)/2</f>
         <v>0.46666666666666667</v>
       </c>
-      <c r="AE36" s="95"/>
-      <c r="AF36" s="104"/>
-      <c r="AG36" s="114"/>
-      <c r="AH36" s="114"/>
-      <c r="AI36" s="105"/>
+      <c r="AE36" s="78"/>
+      <c r="AF36" s="63"/>
+      <c r="AG36" s="73"/>
+      <c r="AH36" s="73"/>
+      <c r="AI36" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="H34:I36"/>
-    <mergeCell ref="P34:Q36"/>
-    <mergeCell ref="X34:Y36"/>
-    <mergeCell ref="AF34:AI36"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="L36:M36"/>
-    <mergeCell ref="N36:O36"/>
-    <mergeCell ref="R36:S36"/>
-    <mergeCell ref="T36:U36"/>
-    <mergeCell ref="V36:W36"/>
-    <mergeCell ref="Z36:AA36"/>
-    <mergeCell ref="AB36:AC36"/>
-    <mergeCell ref="AD36:AE36"/>
-    <mergeCell ref="J1:Q1"/>
     <mergeCell ref="R1:Y1"/>
     <mergeCell ref="AH1:AH3"/>
     <mergeCell ref="AI1:AI3"/>
@@ -28650,6 +28631,25 @@
     <mergeCell ref="Z1:AG1"/>
     <mergeCell ref="Z2:AA2"/>
     <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="H34:I36"/>
+    <mergeCell ref="P34:Q36"/>
+    <mergeCell ref="X34:Y36"/>
+    <mergeCell ref="AF34:AI36"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="R36:S36"/>
+    <mergeCell ref="T36:U36"/>
+    <mergeCell ref="V36:W36"/>
+    <mergeCell ref="Z36:AA36"/>
+    <mergeCell ref="AB36:AC36"/>
+    <mergeCell ref="AD36:AE36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28706,113 +28706,113 @@
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A1" s="22"/>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
-      <c r="H1" s="63"/>
-      <c r="I1" s="63"/>
-      <c r="J1" s="64" t="s">
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="90"/>
+      <c r="I1" s="90"/>
+      <c r="J1" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
-      <c r="O1" s="64"/>
-      <c r="P1" s="64"/>
-      <c r="Q1" s="64"/>
-      <c r="R1" s="65" t="s">
+      <c r="K1" s="91"/>
+      <c r="L1" s="91"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="91"/>
+      <c r="O1" s="91"/>
+      <c r="P1" s="91"/>
+      <c r="Q1" s="91"/>
+      <c r="R1" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="65"/>
-      <c r="T1" s="65"/>
-      <c r="U1" s="65"/>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="62" t="s">
+      <c r="S1" s="92"/>
+      <c r="T1" s="92"/>
+      <c r="U1" s="92"/>
+      <c r="V1" s="92"/>
+      <c r="W1" s="92"/>
+      <c r="X1" s="92"/>
+      <c r="Y1" s="92"/>
+      <c r="Z1" s="102" t="s">
         <v>75</v>
       </c>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62"/>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
-      <c r="AE1" s="62"/>
-      <c r="AF1" s="62"/>
-      <c r="AG1" s="62"/>
-      <c r="AH1" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI1" s="59" t="s">
+      <c r="AA1" s="102"/>
+      <c r="AB1" s="102"/>
+      <c r="AC1" s="102"/>
+      <c r="AD1" s="102"/>
+      <c r="AE1" s="102"/>
+      <c r="AF1" s="102"/>
+      <c r="AG1" s="102"/>
+      <c r="AH1" s="99" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI1" s="99" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A2" s="22"/>
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="93" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="66" t="s">
+      <c r="C2" s="94"/>
+      <c r="D2" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="67"/>
-      <c r="F2" s="66" t="s">
+      <c r="E2" s="94"/>
+      <c r="F2" s="93" t="s">
         <v>49</v>
       </c>
-      <c r="G2" s="67"/>
+      <c r="G2" s="94"/>
       <c r="H2" s="24"/>
       <c r="I2" s="24"/>
-      <c r="J2" s="68" t="s">
+      <c r="J2" s="95" t="s">
         <v>50</v>
       </c>
-      <c r="K2" s="69"/>
-      <c r="L2" s="68" t="s">
+      <c r="K2" s="96"/>
+      <c r="L2" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="M2" s="69"/>
-      <c r="N2" s="68" t="s">
+      <c r="M2" s="96"/>
+      <c r="N2" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="O2" s="69"/>
+      <c r="O2" s="96"/>
       <c r="P2" s="25"/>
       <c r="Q2" s="25"/>
-      <c r="R2" s="70" t="s">
+      <c r="R2" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="S2" s="71"/>
-      <c r="T2" s="70" t="s">
+      <c r="S2" s="98"/>
+      <c r="T2" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="U2" s="71"/>
-      <c r="V2" s="70" t="s">
+      <c r="U2" s="98"/>
+      <c r="V2" s="97" t="s">
         <v>55</v>
       </c>
-      <c r="W2" s="71"/>
+      <c r="W2" s="98"/>
       <c r="X2" s="26"/>
       <c r="Y2" s="26"/>
-      <c r="Z2" s="60" t="s">
+      <c r="Z2" s="100" t="s">
         <v>47</v>
       </c>
-      <c r="AA2" s="61"/>
-      <c r="AB2" s="60" t="s">
+      <c r="AA2" s="101"/>
+      <c r="AB2" s="100" t="s">
         <v>48</v>
       </c>
-      <c r="AC2" s="61"/>
-      <c r="AD2" s="60" t="s">
+      <c r="AC2" s="101"/>
+      <c r="AD2" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="AE2" s="61"/>
+      <c r="AE2" s="101"/>
       <c r="AF2" s="18"/>
       <c r="AG2" s="18"/>
-      <c r="AH2" s="59"/>
-      <c r="AI2" s="59"/>
+      <c r="AH2" s="99"/>
+      <c r="AI2" s="99"/>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
@@ -28914,8 +28914,8 @@
       <c r="AG3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="AH3" s="59"/>
-      <c r="AI3" s="59"/>
+      <c r="AH3" s="99"/>
+      <c r="AI3" s="99"/>
       <c r="AK3" s="22" t="s">
         <v>83</v>
       </c>
@@ -32565,8 +32565,8 @@
         <f>SUM(G4:G33)</f>
         <v>18</v>
       </c>
-      <c r="H34" s="100"/>
-      <c r="I34" s="101"/>
+      <c r="H34" s="59"/>
+      <c r="I34" s="60"/>
       <c r="J34" s="46">
         <f t="shared" ref="J34:O34" si="11">SUM(J4:J33)</f>
         <v>16</v>
@@ -32591,8 +32591,8 @@
         <f t="shared" si="11"/>
         <v>18</v>
       </c>
-      <c r="P34" s="106"/>
-      <c r="Q34" s="107"/>
+      <c r="P34" s="65"/>
+      <c r="Q34" s="66"/>
       <c r="R34" s="47">
         <f>SUM(R4:R33)</f>
         <v>19</v>
@@ -32617,8 +32617,8 @@
         <f>SUM(W4:W33)</f>
         <v>14</v>
       </c>
-      <c r="X34" s="106"/>
-      <c r="Y34" s="107"/>
+      <c r="X34" s="65"/>
+      <c r="Y34" s="66"/>
       <c r="Z34" s="45">
         <f>SUM(Z4:Z33)</f>
         <v>21</v>
@@ -32643,199 +32643,217 @@
         <f>SUM(AE4:AE33)</f>
         <v>17</v>
       </c>
-      <c r="AF34" s="100"/>
-      <c r="AG34" s="112"/>
-      <c r="AH34" s="112"/>
-      <c r="AI34" s="101"/>
+      <c r="AF34" s="59"/>
+      <c r="AG34" s="71"/>
+      <c r="AH34" s="71"/>
+      <c r="AI34" s="60"/>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A35" s="93" t="s">
+      <c r="A35" s="58" t="s">
         <v>99</v>
       </c>
-      <c r="B35" s="89">
+      <c r="B35" s="54">
         <f>B34/$A$33</f>
         <v>0.7</v>
       </c>
-      <c r="C35" s="89">
+      <c r="C35" s="54">
         <f t="shared" ref="C35:G35" si="14">C34/$A$33</f>
         <v>0.6333333333333333</v>
       </c>
-      <c r="D35" s="89">
+      <c r="D35" s="54">
         <f t="shared" si="14"/>
         <v>0.6</v>
       </c>
-      <c r="E35" s="89">
+      <c r="E35" s="54">
         <f t="shared" si="14"/>
         <v>0.56666666666666665</v>
       </c>
-      <c r="F35" s="89">
+      <c r="F35" s="54">
         <f t="shared" si="14"/>
         <v>0.76666666666666672</v>
       </c>
-      <c r="G35" s="89">
+      <c r="G35" s="54">
         <f t="shared" si="14"/>
         <v>0.6</v>
       </c>
-      <c r="H35" s="102"/>
-      <c r="I35" s="103"/>
-      <c r="J35" s="91">
-        <f>J34/$A$33</f>
+      <c r="H35" s="61"/>
+      <c r="I35" s="62"/>
+      <c r="J35" s="56">
+        <f t="shared" ref="J35:O35" si="15">J34/$A$33</f>
         <v>0.53333333333333333</v>
       </c>
-      <c r="K35" s="91">
-        <f>K34/$A$33</f>
+      <c r="K35" s="56">
+        <f t="shared" si="15"/>
         <v>0.6333333333333333</v>
       </c>
-      <c r="L35" s="91">
-        <f>L34/$A$33</f>
+      <c r="L35" s="56">
+        <f t="shared" si="15"/>
         <v>0.56666666666666665</v>
       </c>
-      <c r="M35" s="91">
-        <f>M34/$A$33</f>
+      <c r="M35" s="56">
+        <f t="shared" si="15"/>
         <v>0.5</v>
       </c>
-      <c r="N35" s="91">
-        <f>N34/$A$33</f>
+      <c r="N35" s="56">
+        <f t="shared" si="15"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="O35" s="91">
-        <f>O34/$A$33</f>
+      <c r="O35" s="56">
+        <f t="shared" si="15"/>
         <v>0.6</v>
       </c>
-      <c r="P35" s="108"/>
-      <c r="Q35" s="109"/>
-      <c r="R35" s="92">
-        <f>R34/$A$33</f>
+      <c r="P35" s="67"/>
+      <c r="Q35" s="68"/>
+      <c r="R35" s="57">
+        <f t="shared" ref="R35:W35" si="16">R34/$A$33</f>
         <v>0.6333333333333333</v>
       </c>
-      <c r="S35" s="92">
-        <f>S34/$A$33</f>
+      <c r="S35" s="57">
+        <f t="shared" si="16"/>
         <v>0.7</v>
       </c>
-      <c r="T35" s="92">
-        <f>T34/$A$33</f>
+      <c r="T35" s="57">
+        <f t="shared" si="16"/>
         <v>0.7</v>
       </c>
-      <c r="U35" s="92">
-        <f>U34/$A$33</f>
+      <c r="U35" s="57">
+        <f t="shared" si="16"/>
         <v>0.5</v>
       </c>
-      <c r="V35" s="92">
-        <f>V34/$A$33</f>
+      <c r="V35" s="57">
+        <f t="shared" si="16"/>
         <v>0.7</v>
       </c>
-      <c r="W35" s="92">
-        <f>W34/$A$33</f>
+      <c r="W35" s="57">
+        <f t="shared" si="16"/>
         <v>0.46666666666666667</v>
       </c>
-      <c r="X35" s="108"/>
-      <c r="Y35" s="109"/>
-      <c r="Z35" s="89">
-        <f>Z34/$A$33</f>
+      <c r="X35" s="67"/>
+      <c r="Y35" s="68"/>
+      <c r="Z35" s="54">
+        <f t="shared" ref="Z35:AE35" si="17">Z34/$A$33</f>
         <v>0.7</v>
       </c>
-      <c r="AA35" s="89">
-        <f>AA34/$A$33</f>
+      <c r="AA35" s="54">
+        <f t="shared" si="17"/>
         <v>0.8666666666666667</v>
       </c>
-      <c r="AB35" s="89">
-        <f>AB34/$A$33</f>
+      <c r="AB35" s="54">
+        <f t="shared" si="17"/>
         <v>0.4</v>
       </c>
-      <c r="AC35" s="89">
-        <f>AC34/$A$33</f>
+      <c r="AC35" s="54">
+        <f t="shared" si="17"/>
         <v>0.6333333333333333</v>
       </c>
-      <c r="AD35" s="89">
-        <f>AD34/$A$33</f>
+      <c r="AD35" s="54">
+        <f t="shared" si="17"/>
         <v>0.6</v>
       </c>
-      <c r="AE35" s="89">
-        <f>AE34/$A$33</f>
+      <c r="AE35" s="54">
+        <f t="shared" si="17"/>
         <v>0.56666666666666665</v>
       </c>
-      <c r="AF35" s="102"/>
-      <c r="AG35" s="113"/>
-      <c r="AH35" s="113"/>
-      <c r="AI35" s="103"/>
+      <c r="AF35" s="61"/>
+      <c r="AG35" s="72"/>
+      <c r="AH35" s="72"/>
+      <c r="AI35" s="62"/>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B36" s="94">
+      <c r="B36" s="77">
         <f>(B35+C35)/2</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="C36" s="95"/>
-      <c r="D36" s="94">
+      <c r="C36" s="78"/>
+      <c r="D36" s="77">
         <f>(D35+E35)/2</f>
         <v>0.58333333333333326</v>
       </c>
-      <c r="E36" s="95"/>
-      <c r="F36" s="94">
+      <c r="E36" s="78"/>
+      <c r="F36" s="77">
         <f>(F35+G35)/2</f>
         <v>0.68333333333333335</v>
       </c>
-      <c r="G36" s="95"/>
-      <c r="H36" s="104"/>
-      <c r="I36" s="105"/>
-      <c r="J36" s="96">
+      <c r="G36" s="78"/>
+      <c r="H36" s="63"/>
+      <c r="I36" s="64"/>
+      <c r="J36" s="79">
         <f>(J35+K35)/2</f>
         <v>0.58333333333333326</v>
       </c>
-      <c r="K36" s="97"/>
-      <c r="L36" s="96">
+      <c r="K36" s="80"/>
+      <c r="L36" s="79">
         <f>(L35+M35)/2</f>
         <v>0.53333333333333333</v>
       </c>
-      <c r="M36" s="97"/>
-      <c r="N36" s="96">
+      <c r="M36" s="80"/>
+      <c r="N36" s="79">
         <f>(N35+O35)/2</f>
         <v>0.6333333333333333</v>
       </c>
-      <c r="O36" s="97"/>
-      <c r="P36" s="110"/>
-      <c r="Q36" s="111"/>
-      <c r="R36" s="98">
+      <c r="O36" s="80"/>
+      <c r="P36" s="69"/>
+      <c r="Q36" s="70"/>
+      <c r="R36" s="81">
         <f>(R35+S35)/2</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="S36" s="99"/>
-      <c r="T36" s="98">
+      <c r="S36" s="82"/>
+      <c r="T36" s="81">
         <f>(T35+U35)/2</f>
         <v>0.6</v>
       </c>
-      <c r="U36" s="99"/>
-      <c r="V36" s="98">
+      <c r="U36" s="82"/>
+      <c r="V36" s="81">
         <f>(V35+W35)/2</f>
         <v>0.58333333333333326</v>
       </c>
-      <c r="W36" s="99"/>
-      <c r="X36" s="110"/>
-      <c r="Y36" s="111"/>
-      <c r="Z36" s="94">
+      <c r="W36" s="82"/>
+      <c r="X36" s="69"/>
+      <c r="Y36" s="70"/>
+      <c r="Z36" s="77">
         <f>(Z35+AA35)/2</f>
         <v>0.78333333333333333</v>
       </c>
-      <c r="AA36" s="95"/>
-      <c r="AB36" s="94">
+      <c r="AA36" s="78"/>
+      <c r="AB36" s="77">
         <f>(AB35+AC35)/2</f>
         <v>0.51666666666666661</v>
       </c>
-      <c r="AC36" s="95"/>
-      <c r="AD36" s="94">
+      <c r="AC36" s="78"/>
+      <c r="AD36" s="77">
         <f>(AD35+AE35)/2</f>
         <v>0.58333333333333326</v>
       </c>
-      <c r="AE36" s="95"/>
-      <c r="AF36" s="104"/>
-      <c r="AG36" s="114"/>
-      <c r="AH36" s="114"/>
-      <c r="AI36" s="105"/>
+      <c r="AE36" s="78"/>
+      <c r="AF36" s="63"/>
+      <c r="AG36" s="73"/>
+      <c r="AH36" s="73"/>
+      <c r="AI36" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="AH1:AH3"/>
+    <mergeCell ref="AI1:AI3"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="AB2:AC2"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="Z1:AG1"/>
+    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="J1:Q1"/>
+    <mergeCell ref="R1:Y1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
     <mergeCell ref="H34:I36"/>
     <mergeCell ref="P34:Q36"/>
     <mergeCell ref="X34:Y36"/>
@@ -32852,24 +32870,6 @@
     <mergeCell ref="Z36:AA36"/>
     <mergeCell ref="AB36:AC36"/>
     <mergeCell ref="AD36:AE36"/>
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="R1:Y1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="L2:M2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="AH1:AH3"/>
-    <mergeCell ref="AI1:AI3"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AC2"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="Z1:AG1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -32879,7 +32879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D57"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M57" sqref="M57"/>
     </sheetView>
   </sheetViews>
@@ -32889,11 +32889,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="102" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="62"/>
-      <c r="D2" s="62"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="48"/>
@@ -32944,23 +32944,23 @@
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="75" t="s">
+      <c r="B17" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="76"/>
-      <c r="D17" s="77"/>
+      <c r="C17" s="104"/>
+      <c r="D17" s="105"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="78"/>
-      <c r="C18" s="78" t="s">
+      <c r="B18" s="49"/>
+      <c r="C18" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="78" t="s">
+      <c r="D18" s="49" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="79" t="s">
+      <c r="B19" s="50" t="s">
         <v>50</v>
       </c>
       <c r="C19" s="11">
@@ -32973,7 +32973,7 @@
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="79" t="s">
+      <c r="B20" s="50" t="s">
         <v>51</v>
       </c>
       <c r="C20" s="11">
@@ -32986,7 +32986,7 @@
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="79" t="s">
+      <c r="B21" s="50" t="s">
         <v>52</v>
       </c>
       <c r="C21" s="11">
@@ -32999,23 +32999,23 @@
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="80" t="s">
+      <c r="B34" s="106" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="81"/>
-      <c r="D34" s="82"/>
+      <c r="C34" s="107"/>
+      <c r="D34" s="108"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" s="83"/>
-      <c r="C35" s="83" t="s">
+      <c r="B35" s="51"/>
+      <c r="C35" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="D35" s="83" t="s">
+      <c r="D35" s="51" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" s="84" t="s">
+      <c r="B36" s="52" t="s">
         <v>53</v>
       </c>
       <c r="C36" s="11">
@@ -33028,7 +33028,7 @@
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" s="84" t="s">
+      <c r="B37" s="52" t="s">
         <v>54</v>
       </c>
       <c r="C37" s="11">
@@ -33041,7 +33041,7 @@
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" s="84" t="s">
+      <c r="B38" s="52" t="s">
         <v>55</v>
       </c>
       <c r="C38" s="11">
@@ -33054,23 +33054,23 @@
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B53" s="85" t="s">
+      <c r="B53" s="109" t="s">
         <v>94</v>
       </c>
-      <c r="C53" s="86"/>
-      <c r="D53" s="87"/>
+      <c r="C53" s="110"/>
+      <c r="D53" s="111"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B54" s="88"/>
-      <c r="C54" s="88" t="s">
+      <c r="B54" s="53"/>
+      <c r="C54" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="D54" s="88" t="s">
+      <c r="D54" s="53" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B55" s="79" t="s">
+      <c r="B55" s="50" t="s">
         <v>96</v>
       </c>
       <c r="C55" s="11">
@@ -33083,7 +33083,7 @@
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B56" s="79" t="s">
+      <c r="B56" s="50" t="s">
         <v>97</v>
       </c>
       <c r="C56" s="11">
@@ -33096,7 +33096,7 @@
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B57" s="79" t="s">
+      <c r="B57" s="50" t="s">
         <v>98</v>
       </c>
       <c r="C57" s="11">
@@ -33124,7 +33124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y51"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="H21" workbookViewId="0">
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
@@ -33136,15 +33136,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="112" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="73"/>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="74"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="114"/>
       <c r="V2" s="1"/>
       <c r="W2" s="5" t="s">
         <v>5</v>
@@ -33435,15 +33435,15 @@
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="112" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="73"/>
-      <c r="C13" s="73"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="73"/>
-      <c r="F13" s="73"/>
-      <c r="G13" s="74"/>
+      <c r="B13" s="113"/>
+      <c r="C13" s="113"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="114"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
@@ -33563,15 +33563,15 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="72" t="s">
+      <c r="A24" s="112" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="73"/>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="74"/>
+      <c r="B24" s="113"/>
+      <c r="C24" s="113"/>
+      <c r="D24" s="113"/>
+      <c r="E24" s="113"/>
+      <c r="F24" s="113"/>
+      <c r="G24" s="114"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
@@ -33690,16 +33690,16 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="72" t="s">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" s="112" t="s">
         <v>94</v>
       </c>
-      <c r="B35" s="73"/>
-      <c r="C35" s="73"/>
-      <c r="D35" s="73"/>
-      <c r="E35" s="73"/>
-      <c r="F35" s="73"/>
-      <c r="G35" s="74"/>
+      <c r="B35" s="113"/>
+      <c r="C35" s="113"/>
+      <c r="D35" s="113"/>
+      <c r="E35" s="113"/>
+      <c r="F35" s="113"/>
+      <c r="G35" s="114"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
@@ -33819,15 +33819,15 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46" s="72" t="s">
+      <c r="A46" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="B46" s="73"/>
-      <c r="C46" s="73"/>
-      <c r="D46" s="73"/>
-      <c r="E46" s="73"/>
-      <c r="F46" s="73"/>
-      <c r="G46" s="74"/>
+      <c r="B46" s="113"/>
+      <c r="C46" s="113"/>
+      <c r="D46" s="113"/>
+      <c r="E46" s="113"/>
+      <c r="F46" s="113"/>
+      <c r="G46" s="114"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="19" t="s">
@@ -34566,8 +34566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34908,7 +34908,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>

</xml_diff>